<commit_message>
refactor: SEO audit & rapport opti
</commit_message>
<xml_diff>
--- a/P4_01_analyse.xlsx
+++ b/P4_01_analyse.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>Catégorie</t>
   </si>
@@ -1797,6 +1797,82 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> des images ne décrit pas correctement les images et dégrade fortement l'accessibilité aux personnes qui utilisent un lecteur d'écran ou qui ont une connexion lente.</t>
+    </r>
+  </si>
+  <si>
+    <t>Les éléments d'en-tête ne sont pas dans un ordre séquentiel décroissant</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/HTML/Element/Heading_Elements</t>
+  </si>
+  <si>
+    <r>
+      <t>On évitera de sauter des niveaux de titre : on commence toujours par</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;h1&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> puis </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;h2&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> et ainsi de suite. On essaye également d'avoir un seul titre de niveau 1 sur une page. Jusqu'à HTML5, il fallait éviter d'utiliser plus d'un élément &lt;h1&gt; sur une même page. En HTML5, il est possible d'utiliser les balises sémantiques pour créer une hiérarchie valide avec plusieurs </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;h1&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> les éléments de titre de section 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;h1&gt;-&lt;h6&gt;</t>
     </r>
   </si>
 </sst>
@@ -2176,10 +2252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z991"/>
+  <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2413,117 +2489,121 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="123" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:26" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="12"/>
+      <c r="G14" s="12"/>
     </row>
-    <row r="14" spans="1:26" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+    <row r="15" spans="1:26" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="3" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="166.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="16" spans="1:26" ht="166.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="3" t="s">
+      <c r="E16" s="10"/>
+      <c r="F16" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2570,7 +2650,14 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3538,22 +3625,24 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F9" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F13" r:id="rId3"/>
+    <hyperlink ref="F14" r:id="rId3"/>
     <hyperlink ref="F4" r:id="rId4"/>
-    <hyperlink ref="F12" r:id="rId5"/>
+    <hyperlink ref="F13" r:id="rId5"/>
     <hyperlink ref="F8" r:id="rId6"/>
-    <hyperlink ref="F15" r:id="rId7" location="fallbacks"/>
+    <hyperlink ref="F16" r:id="rId7" location="fallbacks"/>
     <hyperlink ref="F7" r:id="rId8"/>
     <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F11" r:id="rId10" location="label-buttons-and-links"/>
+    <hyperlink ref="F12" r:id="rId10" location="label-buttons-and-links"/>
     <hyperlink ref="F5" r:id="rId11"/>
     <hyperlink ref="F6" r:id="rId12" display="https://blog.logrocket.com/the-complete-best-practices-for-minifying-css/"/>
+    <hyperlink ref="F11" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId13"/>
+  <pageSetup orientation="landscape" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: repport & SEO audit
</commit_message>
<xml_diff>
--- a/P4_01_analyse.xlsx
+++ b/P4_01_analyse.xlsx
@@ -2254,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>